<commit_message>
Initial protected feature imputation
Note: CatBoost needs to be installed to run infer_protected.ipynb.
</commit_message>
<xml_diff>
--- a/SIOP ML - 2020-03-16 - Analytical work process.xlsx
+++ b/SIOP ML - 2020-03-16 - Analytical work process.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Goran\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robinburke/Documents/GitHub/POIS-0202-Moixa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3B44B7-4E2C-4B19-8027-3FE6A68D2B0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E3A6D2-0CA6-2049-9D0C-F9A3F1343282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F2833F91-EEE0-4421-AB7B-DD20B8760460}"/>
+    <workbookView xWindow="4740" yWindow="2160" windowWidth="19420" windowHeight="10420" xr2:uid="{F2833F91-EEE0-4421-AB7B-DD20B8760460}"/>
   </bookViews>
   <sheets>
     <sheet name="Data exploration" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>Ignored missing values; factor analysis on personality items extracting 13 factors used only to predict High_Perfomer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Protected feature</t>
+  </si>
+  <si>
+    <t>Burke</t>
+  </si>
+  <si>
+    <t>1st pass</t>
+  </si>
+  <si>
+    <t>With bio data only, about 70% accuracy is achieved across different classifiers.</t>
   </si>
 </sst>
 </file>
@@ -565,27 +577,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5BA4D9-CD12-42F3-9AE5-071AFA9AA84F}">
-  <dimension ref="B1:F11"/>
+  <dimension ref="B1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.81640625" customWidth="1"/>
-    <col min="2" max="2" width="35.81640625" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" customWidth="1"/>
+    <col min="1" max="1" width="1.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="26.54296875" customWidth="1"/>
-    <col min="6" max="6" width="43.7265625" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="6.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="2:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
@@ -602,7 +614,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
@@ -611,7 +623,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -622,7 +634,7 @@
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -633,7 +645,7 @@
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -644,7 +656,7 @@
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -655,7 +667,7 @@
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
@@ -664,7 +676,7 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -673,7 +685,7 @@
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -682,7 +694,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -690,6 +702,20 @@
       <c r="D11" s="19"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -706,31 +732,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287C6F7C-3129-46F4-9567-AA9B5957D940}">
   <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.453125" customWidth="1"/>
-    <col min="2" max="2" width="48.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="5" width="18.26953125" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.7265625" customWidth="1"/>
+    <col min="1" max="1" width="1.5" customWidth="1"/>
+    <col min="2" max="2" width="48.5" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C2" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
     </row>
-    <row r="3" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
@@ -756,7 +782,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
@@ -779,7 +805,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
@@ -805,7 +831,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -817,7 +843,7 @@
       <c r="H6" s="15"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
@@ -829,22 +855,22 @@
       <c r="H7" s="15"/>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>

</xml_diff>